<commit_message>
modified:   "f\303\251l\303\251ves_jav\303\255t\303\241s/Parallel.xlsx" 	modified:   "f\303\251l\303\251ves_jav\303\255t\303\241s/opencl/makefile" 	modified:   "f\303\251l\303\251ves_jav\303\255t\303\241s/opencl/matrix_addition.c" 	modified:   "f\303\251l\303\251ves_jav\303\255t\303\241s/openmp/matrix_addition.c" 	modified:   "f\303\251l\303\251ves_jav\303\255t\303\241s/pthread/matrix_addition.c"
</commit_message>
<xml_diff>
--- a/féléves_javítás/Parallel.xlsx
+++ b/féléves_javítás/Parallel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rebuu\Desktop\Suli\Parallel\parallel\féléves_javítás\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF10C59-5DC5-45BE-8A53-330CE7CFB05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2D7027-794D-41D3-BDAD-5CB48BCD36A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -244,44 +244,6 @@
       </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
-    <c:view3D>
-      <c:rotX val="15"/>
-      <c:rotY val="20"/>
-      <c:rAngAx val="0"/>
-    </c:view3D>
-    <c:floor>
-      <c:thickness val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:sp3d/>
-      </c:spPr>
-    </c:floor>
-    <c:sideWall>
-      <c:thickness val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:sp3d/>
-      </c:spPr>
-    </c:sideWall>
-    <c:backWall>
-      <c:thickness val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:sp3d/>
-      </c:spPr>
-    </c:backWall>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -294,7 +256,7 @@
           <c:h val="0.60615632612519632"/>
         </c:manualLayout>
       </c:layout>
-      <c:bar3DChart>
+      <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
@@ -320,7 +282,6 @@
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
-            <a:sp3d/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -488,7 +449,6 @@
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
-            <a:sp3d/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -656,7 +616,6 @@
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
-            <a:sp3d/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -734,64 +693,64 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1.853356</c:v>
+                  <c:v>0.49505399999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1457619999999999</c:v>
+                  <c:v>0.49049399999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.145637</c:v>
+                  <c:v>0.48364099999999999</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>1.9376420000000001</c:v>
+                  <c:v>0.39807799999999999</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>1.837674</c:v>
+                  <c:v>0.40021600000000002</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="General">
-                  <c:v>1.146028</c:v>
+                  <c:v>0.383185</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
-                  <c:v>1.145416</c:v>
+                  <c:v>0.40973799999999999</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
-                  <c:v>1.1788099999999999</c:v>
+                  <c:v>0.37506200000000001</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="General">
-                  <c:v>1.145618</c:v>
+                  <c:v>0.38073499999999999</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
-                  <c:v>1.145734</c:v>
+                  <c:v>0.37915199999999999</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="General">
-                  <c:v>1.1304190000000001</c:v>
+                  <c:v>0.37596600000000002</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="General">
-                  <c:v>1.1457790000000001</c:v>
+                  <c:v>0.38241999999999998</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="General">
-                  <c:v>1.145672</c:v>
+                  <c:v>0.384432</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="General">
-                  <c:v>1.1455280000000001</c:v>
+                  <c:v>0.383183</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="General">
-                  <c:v>1.146199</c:v>
+                  <c:v>0.37625900000000001</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="General">
-                  <c:v>1.1460109999999999</c:v>
+                  <c:v>0.37137399999999998</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="General">
-                  <c:v>1.145475</c:v>
+                  <c:v>0.37882199999999999</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="General">
-                  <c:v>1.145675</c:v>
+                  <c:v>0.39555400000000002</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="General">
-                  <c:v>1.1475</c:v>
+                  <c:v>0.37514900000000001</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="General">
-                  <c:v>1.1445399999999999</c:v>
+                  <c:v>0.38949699999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -811,11 +770,9 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:shape val="box"/>
         <c:axId val="1773283839"/>
         <c:axId val="1773285087"/>
-        <c:axId val="0"/>
-      </c:bar3DChart>
+      </c:barChart>
       <c:catAx>
         <c:axId val="1773283839"/>
         <c:scaling>
@@ -871,8 +828,8 @@
         <c:axId val="1773285087"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="2"/>
-          <c:min val="1.1000000000000001"/>
+          <c:max val="1.4"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1055,47 +1012,9 @@
       </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
-    <c:view3D>
-      <c:rotX val="15"/>
-      <c:rotY val="20"/>
-      <c:rAngAx val="0"/>
-    </c:view3D>
-    <c:floor>
-      <c:thickness val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:sp3d/>
-      </c:spPr>
-    </c:floor>
-    <c:sideWall>
-      <c:thickness val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:sp3d/>
-      </c:spPr>
-    </c:sideWall>
-    <c:backWall>
-      <c:thickness val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:sp3d/>
-      </c:spPr>
-    </c:backWall>
     <c:plotArea>
       <c:layout/>
-      <c:bar3DChart>
+      <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
@@ -1121,7 +1040,6 @@
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
-            <a:sp3d/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:val>
@@ -1206,7 +1124,6 @@
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
-            <a:sp3d/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:val>
@@ -1291,7 +1208,6 @@
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
-            <a:sp3d/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:val>
@@ -1301,49 +1217,49 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>1.3515779999999999</c:v>
+                  <c:v>0.124069</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.67528999999999995</c:v>
+                  <c:v>0.12784899999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.67532899999999996</c:v>
+                  <c:v>0.13491800000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.70435000000000003</c:v>
+                  <c:v>0.14202500000000001</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>0.70264599999999999</c:v>
+                  <c:v>0.148592</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="General">
-                  <c:v>0.736985</c:v>
+                  <c:v>0.179539</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
-                  <c:v>0.75336700000000001</c:v>
+                  <c:v>0.19530500000000001</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
-                  <c:v>0.796678</c:v>
+                  <c:v>0.22969400000000001</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="General">
-                  <c:v>0.82289900000000005</c:v>
+                  <c:v>0.25361400000000001</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
-                  <c:v>0.86430700000000005</c:v>
+                  <c:v>0.28656900000000002</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="General">
-                  <c:v>0.924369</c:v>
+                  <c:v>0.31492399999999998</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="General">
-                  <c:v>0.97381499999999999</c:v>
+                  <c:v>0.35635699999999998</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="General">
-                  <c:v>1.0200070000000001</c:v>
+                  <c:v>0.39061000000000001</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="General">
-                  <c:v>1.084066</c:v>
+                  <c:v>0.43513800000000002</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="General">
-                  <c:v>1.1770640000000001</c:v>
+                  <c:v>0.481097</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1363,11 +1279,9 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:shape val="box"/>
         <c:axId val="71239487"/>
         <c:axId val="71240735"/>
-        <c:axId val="0"/>
-      </c:bar3DChart>
+      </c:barChart>
       <c:catAx>
         <c:axId val="71239487"/>
         <c:scaling>
@@ -3013,7 +2927,7 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="D24" sqref="D24:D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3050,7 +2964,7 @@
         <v>1.334525</v>
       </c>
       <c r="D2" s="2">
-        <v>1.853356</v>
+        <v>0.49505399999999999</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -3064,7 +2978,7 @@
         <v>1.38178</v>
       </c>
       <c r="D3" s="2">
-        <v>1.1457619999999999</v>
+        <v>0.49049399999999999</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -3078,7 +2992,7 @@
         <v>1.3485290000000001</v>
       </c>
       <c r="D4" s="2">
-        <v>1.145637</v>
+        <v>0.48364099999999999</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -3092,7 +3006,7 @@
         <v>1.351831</v>
       </c>
       <c r="D5" s="1">
-        <v>1.9376420000000001</v>
+        <v>0.39807799999999999</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -3106,7 +3020,7 @@
         <v>1.3509230000000001</v>
       </c>
       <c r="D6" s="1">
-        <v>1.837674</v>
+        <v>0.40021600000000002</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -3120,7 +3034,7 @@
         <v>1.317761</v>
       </c>
       <c r="D7" s="1">
-        <v>1.146028</v>
+        <v>0.383185</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -3134,7 +3048,7 @@
         <v>1.333154</v>
       </c>
       <c r="D8" s="1">
-        <v>1.145416</v>
+        <v>0.40973799999999999</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -3148,7 +3062,7 @@
         <v>1.3341860000000001</v>
       </c>
       <c r="D9" s="1">
-        <v>1.1788099999999999</v>
+        <v>0.37506200000000001</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -3162,7 +3076,7 @@
         <v>1.34887</v>
       </c>
       <c r="D10" s="1">
-        <v>1.145618</v>
+        <v>0.38073499999999999</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -3176,7 +3090,7 @@
         <v>1.3174060000000001</v>
       </c>
       <c r="D11" s="1">
-        <v>1.145734</v>
+        <v>0.37915199999999999</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -3190,7 +3104,7 @@
         <v>1.3173870000000001</v>
       </c>
       <c r="D12" s="1">
-        <v>1.1304190000000001</v>
+        <v>0.37596600000000002</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -3204,7 +3118,7 @@
         <v>1.33365</v>
       </c>
       <c r="D13" s="1">
-        <v>1.1457790000000001</v>
+        <v>0.38241999999999998</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -3218,7 +3132,7 @@
         <v>1.31745</v>
       </c>
       <c r="D14" s="1">
-        <v>1.145672</v>
+        <v>0.384432</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -3232,7 +3146,7 @@
         <v>1.3335440000000001</v>
       </c>
       <c r="D15" s="1">
-        <v>1.1455280000000001</v>
+        <v>0.383183</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -3246,7 +3160,7 @@
         <v>1.3175330000000001</v>
       </c>
       <c r="D16" s="1">
-        <v>1.146199</v>
+        <v>0.37625900000000001</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -3260,7 +3174,7 @@
         <v>1.318422</v>
       </c>
       <c r="D17" s="1">
-        <v>1.1460109999999999</v>
+        <v>0.37137399999999998</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -3274,7 +3188,7 @@
         <v>1.3030649999999999</v>
       </c>
       <c r="D18" s="1">
-        <v>1.145475</v>
+        <v>0.37882199999999999</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -3288,7 +3202,7 @@
         <v>1.318063</v>
       </c>
       <c r="D19" s="1">
-        <v>1.145675</v>
+        <v>0.39555400000000002</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -3302,7 +3216,7 @@
         <v>1.3179190000000001</v>
       </c>
       <c r="D20" s="1">
-        <v>1.1475</v>
+        <v>0.37514900000000001</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -3316,7 +3230,7 @@
         <v>1.333321</v>
       </c>
       <c r="D21" s="1">
-        <v>1.1445399999999999</v>
+        <v>0.38949699999999998</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -3344,7 +3258,7 @@
         <v>9.9979999999999999E-3</v>
       </c>
       <c r="D24" s="2">
-        <v>1.3515779999999999</v>
+        <v>0.124069</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -3358,7 +3272,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="D25" s="2">
-        <v>0.67528999999999995</v>
+        <v>0.12784899999999999</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -3372,7 +3286,7 @@
         <v>5.7154999999999997E-2</v>
       </c>
       <c r="D26" s="2">
-        <v>0.67532899999999996</v>
+        <v>0.13491800000000001</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -3386,7 +3300,7 @@
         <v>9.7199999999999995E-2</v>
       </c>
       <c r="D27" s="2">
-        <v>0.70435000000000003</v>
+        <v>0.14202500000000001</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -3400,7 +3314,7 @@
         <v>0.15176899999999999</v>
       </c>
       <c r="D28" s="1">
-        <v>0.70264599999999999</v>
+        <v>0.148592</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -3414,7 +3328,7 @@
         <v>0.21462100000000001</v>
       </c>
       <c r="D29" s="1">
-        <v>0.736985</v>
+        <v>0.179539</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -3428,7 +3342,7 @@
         <v>0.28986899999999999</v>
       </c>
       <c r="D30" s="1">
-        <v>0.75336700000000001</v>
+        <v>0.19530500000000001</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -3442,7 +3356,7 @@
         <v>0.37849100000000002</v>
       </c>
       <c r="D31" s="1">
-        <v>0.796678</v>
+        <v>0.22969400000000001</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -3456,7 +3370,7 @@
         <v>0.478437</v>
       </c>
       <c r="D32" s="1">
-        <v>0.82289900000000005</v>
+        <v>0.25361400000000001</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -3470,7 +3384,7 @@
         <v>0.60435700000000003</v>
       </c>
       <c r="D33" s="1">
-        <v>0.86430700000000005</v>
+        <v>0.28656900000000002</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -3484,7 +3398,7 @@
         <v>0.70838000000000001</v>
       </c>
       <c r="D34" s="1">
-        <v>0.924369</v>
+        <v>0.31492399999999998</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -3498,7 +3412,7 @@
         <v>0.84765299999999999</v>
       </c>
       <c r="D35" s="1">
-        <v>0.97381499999999999</v>
+        <v>0.35635699999999998</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -3512,7 +3426,7 @@
         <v>0.99199300000000001</v>
       </c>
       <c r="D36" s="1">
-        <v>1.0200070000000001</v>
+        <v>0.39061000000000001</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -3526,7 +3440,7 @@
         <v>1.148936</v>
       </c>
       <c r="D37" s="1">
-        <v>1.084066</v>
+        <v>0.43513800000000002</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -3540,7 +3454,7 @@
         <v>1.3173569999999999</v>
       </c>
       <c r="D38" s="1">
-        <v>1.1770640000000001</v>
+        <v>0.481097</v>
       </c>
     </row>
   </sheetData>

</xml_diff>